<commit_message>
Changes Made as Requested
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreiHandrau\Documents\GitHub\Revisal_PoC\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreiHandrau\Downloads\Revisal_PoC-Develop (1)\Revisal_PoC-Develop\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4E0FF2-C0D9-4A27-A99F-EF6468FAEF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0997F6BB-51E0-43F5-9755-F8BAE2108EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6975" yWindow="2235" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>C:\Program Files (x86)\TeamNet\ReviSal HG500-2011\teamnet.revisal.ui.exe</t>
+  </si>
+  <si>
+    <t>inputFilePath</t>
+  </si>
+  <si>
+    <t>Data\Input\InputRevisal.xlsx</t>
   </si>
 </sst>
 </file>
@@ -569,7 +575,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -689,7 +695,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>

</xml_diff>